<commit_message>
[Feat] Player, Weapon BGDatabase -> SO 전환 구현 및 플레이어, 무기 스텟 수치 적용
</commit_message>
<xml_diff>
--- a/Assets/Data/GameDB.xlsx
+++ b/Assets/Data/GameDB.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fork\Last-Rites\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3184571-9D3B-4323-9E74-D01F5454A4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEBCBDE-58CA-4F7D-91AB-322FCF0A193A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GameDB" sheetId="1" r:id="rId1"/>
+    <sheet name="Player" sheetId="1" r:id="rId1"/>
+    <sheet name="Weapon" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,12 +37,146 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dash_Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Move_Spd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dash_Spd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dash_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max_Stamina</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stamina_Regen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dash_Cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장의사</t>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Atk_Spd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combo_1</t>
+  </si>
+  <si>
+    <t>Combo_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combo_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q_Dmg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W_Dmg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_Dmg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V_Dmg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>철의 처녀</t>
+  </si>
+  <si>
+    <t>망자 향로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사슬 낫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영혼 랜턴</t>
+  </si>
+  <si>
+    <t>GreatSword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hammer</t>
+  </si>
+  <si>
+    <t>DualBlade</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>R_Val</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WeaponID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +189,15 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -80,9 +224,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,14 +568,372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF11" sqref="AF11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.9140625" customWidth="1"/>
+    <col min="7" max="7" width="12.08203125" customWidth="1"/>
+    <col min="8" max="8" width="12.4140625" customWidth="1"/>
+    <col min="9" max="9" width="13.9140625" customWidth="1"/>
+    <col min="10" max="10" width="10.4140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>0.4</v>
+      </c>
+      <c r="G2">
+        <v>1.5</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.58203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.9140625" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2">
+        <v>0.8</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>40</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>45</v>
+      </c>
+      <c r="M2">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>0.9</v>
+      </c>
+      <c r="O2">
+        <v>15</v>
+      </c>
+      <c r="P2">
+        <v>150</v>
+      </c>
+      <c r="Q2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>0.6</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>40</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>35</v>
+      </c>
+      <c r="K3">
+        <v>12</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3">
+        <v>15</v>
+      </c>
+      <c r="N3">
+        <v>0.5</v>
+      </c>
+      <c r="O3">
+        <v>20</v>
+      </c>
+      <c r="P3">
+        <v>200</v>
+      </c>
+      <c r="Q3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>1.5</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>20</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>25</v>
+      </c>
+      <c r="M4">
+        <v>25</v>
+      </c>
+      <c r="N4">
+        <v>1.3</v>
+      </c>
+      <c r="O4">
+        <v>25</v>
+      </c>
+      <c r="P4">
+        <v>120</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>15</v>
+      </c>
+      <c r="P5">
+        <v>100</v>
+      </c>
+      <c r="Q5">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Feat] AI동료들 SO 구현, AIBase, Actor 겹치는 부분은 통합
</commit_message>
<xml_diff>
--- a/Assets/Data/GameDB.xlsx
+++ b/Assets/Data/GameDB.xlsx
@@ -3,26 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fork\Last-Rites\Assets\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEBCBDE-58CA-4F7D-91AB-322FCF0A193A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
     <sheet name="Weapon" sheetId="2" r:id="rId2"/>
+    <sheet name="AI" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
+    <ext uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures">
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
@@ -37,138 +32,227 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dash_Time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Move_Spd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dash_Spd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dash_Cool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Max_Stamina</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stamina_Regen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dash_Cost</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장의사</t>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Atk_Spd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combo_1</t>
-  </si>
-  <si>
-    <t>Combo_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combo_3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q_Dmg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q_Cool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W_Dmg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W_Cool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E_Dmg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E_Cool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R_Cool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V_Dmg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V_Cool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>철의 처녀</t>
-  </si>
-  <si>
-    <t>망자 향로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사슬 낫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영혼 랜턴</t>
-  </si>
-  <si>
-    <t>GreatSword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hammer</t>
-  </si>
-  <si>
-    <t>DualBlade</t>
-  </si>
-  <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>R_Val</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlayerID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WeaponID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+  <si>
+    <t xml:space="preserve">name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">HP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Dash_Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Move_Spd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Dash_Spd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Dash_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Max_Stamina</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Stamina_Regen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Dash_Cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">장의사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Atk_Spd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Combo_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combo_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Combo_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_Dmg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">W_Dmg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">W_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">E_Dmg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">E_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">R_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">V_Dmg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">V_Cool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">철의 처녀</t>
+  </si>
+  <si>
+    <t xml:space="preserve">망자 향로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">사슬 낫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">영혼 랜턴</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GreatSword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Hammer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DualBlade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_Val</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">PlayerID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">WeaponID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Atk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Val</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Cool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S2_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S2_Val</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S2_Cool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">수호기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">도발</t>
+  </si>
+  <si>
+    <t xml:space="preserve">방패치기</t>
+  </si>
+  <si>
+    <t xml:space="preserve">물의 사제</t>
+  </si>
+  <si>
+    <t xml:space="preserve">치유</t>
+  </si>
+  <si>
+    <t xml:space="preserve">축복</t>
+  </si>
+  <si>
+    <t xml:space="preserve">광전사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">휠윈드</t>
+  </si>
+  <si>
+    <t xml:space="preserve">격분</t>
+  </si>
+  <si>
+    <t xml:space="preserve">그림자 사수</t>
+  </si>
+  <si>
+    <t xml:space="preserve">저격</t>
+  </si>
+  <si>
+    <t xml:space="preserve">덫</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AiID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Healer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Dealer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Respawn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -176,7 +260,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +286,19 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -210,7 +308,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -218,13 +316,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -234,6 +347,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -241,11 +366,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -539,7 +664,7 @@
   <a:objectDefaults>
     <a:lnDef>
       <a:spPr/>
-      <a:bodyPr/>
+      <a:bodyPr rtlCol="0"/>
       <a:lstStyle/>
       <a:style>
         <a:lnRef idx="2">
@@ -567,7 +692,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -654,10 +779,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
@@ -937,4 +1062,213 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>100</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="4">
+        <v>300</v>
+      </c>
+      <c r="E2" s="4">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="4">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="4">
+        <v>2</v>
+      </c>
+      <c r="L2" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>101</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="4">
+        <v>150</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>20</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="4">
+        <v>30</v>
+      </c>
+      <c r="I3" s="4">
+        <v>15</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="4">
+        <v>20</v>
+      </c>
+      <c r="L3" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>102</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="4">
+        <v>200</v>
+      </c>
+      <c r="E4" s="4">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4">
+        <v>20</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="4">
+        <v>12</v>
+      </c>
+      <c r="I4" s="4">
+        <v>10</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="L4" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>103</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="4">
+        <v>120</v>
+      </c>
+      <c r="E5" s="4">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="4">
+        <v>40</v>
+      </c>
+      <c r="I5" s="4">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="4">
+        <v>3</v>
+      </c>
+      <c r="L5" s="4">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>